<commit_message>
EPBDS-7187 EPBDS-9231 More tests
</commit_message>
<xml_diff>
--- a/ITEST/itest.EPBDS-7187/openl-repository/deployments/EPBDS-7187/EPBDS-7187.xlsx
+++ b/ITEST/itest.EPBDS-7187/openl-repository/deployments/EPBDS-7187/EPBDS-7187.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>SimpleRules boolean lowCase(Double number, String string)</t>
   </si>
@@ -89,6 +89,60 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Datatype Mixes</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>aB</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Ba</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>BigDecimal</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>Spreadsheet Mixes mixes(Mixes m)</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>= m</t>
+  </si>
+  <si>
+    <t>= new Mixes[] {m1, m2}</t>
+  </si>
+  <si>
+    <t>Spreadsheet Mixes[] mixes2(Mixes m1, Mixes m2)</t>
   </si>
 </sst>
 </file>
@@ -215,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -230,6 +284,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -602,30 +660,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J25"/>
+  <dimension ref="B3:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" customWidth="1"/>
+    <col min="16" max="16" width="21.85546875" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:17">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
       <c r="H3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="2:10" ht="13.5" thickBot="1">
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" ht="13.5" thickBot="1">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -638,8 +702,14 @@
       <c r="H4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" ht="14.25" thickTop="1" thickBot="1">
+      <c r="O4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -652,16 +722,41 @@
       <c r="H5" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" ht="13.5" thickTop="1"/>
-    <row r="7" spans="2:10">
-      <c r="B7" s="6" t="s">
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="13.5" thickTop="1">
+      <c r="O6" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="2:10" ht="13.5" thickBot="1">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="O7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" ht="13.5" thickBot="1">
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
@@ -671,13 +766,19 @@
       <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="2:10" ht="14.25" thickTop="1" thickBot="1">
+      <c r="O8" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
@@ -693,8 +794,17 @@
       <c r="I9" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" ht="14.25" thickTop="1" thickBot="1">
+      <c r="O9" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9">
+        <v>154.2544</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
       <c r="H10" s="3" t="s">
         <v>4</v>
       </c>
@@ -702,14 +812,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="13.5" thickTop="1">
-      <c r="B11" s="6" t="s">
+    <row r="11" spans="2:17" ht="13.5" thickTop="1">
+      <c r="B11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="2:10" ht="13.5" thickBot="1">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="2:17" ht="13.5" thickBot="1">
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
@@ -720,7 +830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="14.25" thickTop="1" thickBot="1">
+    <row r="13" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
@@ -730,13 +840,13 @@
       <c r="D13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="2:10" ht="14.25" thickTop="1" thickBot="1">
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
       <c r="H14" s="1" t="s">
         <v>1</v>
       </c>
@@ -746,13 +856,17 @@
       <c r="J14" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B15" s="6" t="s">
+      <c r="O14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="P14" s="8"/>
+    </row>
+    <row r="15" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
+      <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
       <c r="H15" s="3" t="s">
         <v>4</v>
       </c>
@@ -762,8 +876,14 @@
       <c r="J15" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" ht="14.25" thickTop="1" thickBot="1">
+      <c r="O15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
@@ -773,8 +893,14 @@
       <c r="D16" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" ht="14.25" thickTop="1" thickBot="1">
+      <c r="O16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P16" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" ht="14.25" thickTop="1" thickBot="1">
       <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
@@ -785,14 +911,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="13.5" thickTop="1">
-      <c r="H18" s="6" t="s">
+    <row r="18" spans="2:16" ht="13.5" thickTop="1">
+      <c r="H18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="2:10" ht="13.5" thickBot="1">
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="2:16" ht="13.5" thickBot="1">
       <c r="H19" s="1" t="s">
         <v>1</v>
       </c>
@@ -803,7 +929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="14.25" thickTop="1" thickBot="1">
+    <row r="20" spans="2:16" ht="14.25" thickTop="1" thickBot="1">
       <c r="H20" s="3" t="s">
         <v>4</v>
       </c>
@@ -813,20 +939,42 @@
       <c r="J20" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="2:10" ht="13.5" thickTop="1"/>
-    <row r="24" spans="2:10">
+      <c r="O20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="P20" s="8"/>
+    </row>
+    <row r="21" spans="2:16" ht="14.25" thickTop="1" thickBot="1">
+      <c r="O21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="14.25" thickTop="1" thickBot="1">
+      <c r="O22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="13.5" thickTop="1"/>
+    <row r="24" spans="2:16">
       <c r="H24" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="2:16">
       <c r="H25" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O20:P20"/>
     <mergeCell ref="H18:J18"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="B3:D3"/>

</xml_diff>

<commit_message>
EPBDS-10365 USE_DEFAULT is not working as designed for nillable fields of Datatypes
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/ITEST/itest.EPBDS-7187/openl-repository/deployments/EPBDS-7187/EPBDS-7187.xlsx
+++ b/ITEST/itest.EPBDS-7187/openl-repository/deployments/EPBDS-7187/EPBDS-7187.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.WebService\openl-repository\EPBDS-7187\EPBDS-7187\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009FD9B6-A2CB-49C9-B92C-4F534AED81E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19635" windowHeight="8190"/>
+    <workbookView xWindow="3280" yWindow="3160" windowWidth="28800" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
   <si>
     <t>SimpleRules boolean lowCase(Double number, String string)</t>
   </si>
@@ -143,12 +149,15 @@
   </si>
   <si>
     <t>Spreadsheet Mixes[] mixes2(Mixes m1, Mixes m2)</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -269,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -284,16 +293,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -369,14 +383,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -414,9 +431,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -449,9 +466,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -484,9 +518,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -659,27 +710,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" customWidth="1"/>
-    <col min="16" max="16" width="21.85546875" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.453125" customWidth="1"/>
+    <col min="16" max="16" width="21.81640625" customWidth="1"/>
+    <col min="17" max="17" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:17">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
       <c r="H3" s="5" t="s">
         <v>18</v>
       </c>
@@ -708,8 +759,11 @@
       <c r="P4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
+      <c r="Q4" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" ht="13.5" thickTop="1" thickBot="1">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -728,31 +782,34 @@
       <c r="P5" t="s">
         <v>10</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:17" ht="13.5" thickTop="1">
+    <row r="6" spans="2:17" ht="13" thickTop="1">
       <c r="O6" t="s">
         <v>28</v>
       </c>
       <c r="P6" t="s">
         <v>29</v>
       </c>
+      <c r="Q6" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:17">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
       <c r="O7" t="s">
         <v>30</v>
       </c>
       <c r="P7" t="s">
         <v>31</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="9">
         <v>43845</v>
       </c>
     </row>
@@ -766,10 +823,10 @@
       <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="5"/>
       <c r="O8" t="s">
         <v>32</v>
@@ -777,8 +834,11 @@
       <c r="P8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
+      <c r="Q8" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="14" thickTop="1" thickBot="1">
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
@@ -800,11 +860,11 @@
       <c r="P9" t="s">
         <v>35</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="8">
         <v>154.2544</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
+    <row r="10" spans="2:17" ht="13.5" thickTop="1" thickBot="1">
       <c r="H10" s="3" t="s">
         <v>4</v>
       </c>
@@ -812,12 +872,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="13.5" thickTop="1">
-      <c r="B11" s="8" t="s">
+    <row r="11" spans="2:17" ht="13" thickTop="1">
+      <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="2:17" ht="13.5" thickBot="1">
       <c r="B12" s="1" t="s">
@@ -830,7 +890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
+    <row r="13" spans="2:17" ht="13.5" thickTop="1" thickBot="1">
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
@@ -840,13 +900,13 @@
       <c r="D13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="2:17" ht="14" thickTop="1" thickBot="1">
       <c r="H14" s="1" t="s">
         <v>1</v>
       </c>
@@ -856,17 +916,17 @@
       <c r="J14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O14" s="8" t="s">
+      <c r="O14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="P14" s="8"/>
-    </row>
-    <row r="15" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B15" s="8" t="s">
+      <c r="P14" s="7"/>
+    </row>
+    <row r="15" spans="2:17" ht="14" thickTop="1" thickBot="1">
+      <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
       <c r="H15" s="3" t="s">
         <v>4</v>
       </c>
@@ -883,7 +943,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="14.25" thickTop="1" thickBot="1">
+    <row r="16" spans="2:17" ht="14" thickTop="1" thickBot="1">
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
@@ -896,11 +956,11 @@
       <c r="O16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="P16" s="7" t="s">
+      <c r="P16" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:16" ht="14.25" thickTop="1" thickBot="1">
+    <row r="17" spans="2:16" ht="13.5" thickTop="1" thickBot="1">
       <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
@@ -911,12 +971,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:16" ht="13.5" thickTop="1">
-      <c r="H18" s="8" t="s">
+    <row r="18" spans="2:16" ht="13" thickTop="1">
+      <c r="H18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="2:16" ht="13.5" thickBot="1">
       <c r="H19" s="1" t="s">
@@ -929,7 +989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:16" ht="14.25" thickTop="1" thickBot="1">
+    <row r="20" spans="2:16" ht="13.5" thickTop="1" thickBot="1">
       <c r="H20" s="3" t="s">
         <v>4</v>
       </c>
@@ -939,12 +999,12 @@
       <c r="J20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O20" s="8" t="s">
+      <c r="O20" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="P20" s="8"/>
-    </row>
-    <row r="21" spans="2:16" ht="14.25" thickTop="1" thickBot="1">
+      <c r="P20" s="7"/>
+    </row>
+    <row r="21" spans="2:16" ht="14" thickTop="1" thickBot="1">
       <c r="O21" s="1" t="s">
         <v>37</v>
       </c>
@@ -952,15 +1012,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="14.25" thickTop="1" thickBot="1">
+    <row r="22" spans="2:16" ht="13.5" thickTop="1" thickBot="1">
       <c r="O22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="P22" s="7" t="s">
+      <c r="P22" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="13.5" thickTop="1"/>
+    <row r="23" spans="2:16" ht="13" thickTop="1"/>
     <row r="24" spans="2:16">
       <c r="H24" s="5" t="s">
         <v>22</v>

</xml_diff>